<commit_message>
Logging und enum in hochkomma.
</commit_message>
<xml_diff>
--- a/src/test/resources/objectimport.xlsx
+++ b/src/test/resources/objectimport.xlsx
@@ -225,7 +225,7 @@
     <t xml:space="preserve">[eins,zwei,drei]</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes,No,Maybe</t>
+    <t xml:space="preserve">Yes,No,0</t>
   </si>
   <si>
     <t xml:space="preserve">Der Array</t>
@@ -520,8 +520,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -736,10 +736,10 @@
         <v>45</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="M7" s="0" t="s">
         <v>46</v>
@@ -782,10 +782,10 @@
         <v>14</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,7 +874,7 @@
         <v>67</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Adding error responses to full crud template.
</commit_message>
<xml_diff>
--- a/src/test/resources/objectimport.xlsx
+++ b/src/test/resources/objectimport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fish" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
   <si>
     <t xml:space="preserve">Position</t>
   </si>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Datentyp</t>
+    <t xml:space="preserve">Datatype</t>
   </si>
   <si>
     <t xml:space="preserve">Nullable</t>
@@ -81,9 +81,6 @@
     <t xml:space="preserve">DBDatatype</t>
   </si>
   <si>
-    <t xml:space="preserve">Datatype</t>
-  </si>
-  <si>
     <t xml:space="preserve">Format</t>
   </si>
   <si>
@@ -219,7 +216,7 @@
     <t xml:space="preserve">acht</t>
   </si>
   <si>
-    <t xml:space="preserve">array</t>
+    <t xml:space="preserve">enum</t>
   </si>
   <si>
     <t xml:space="preserve">[eins,zwei,drei]</t>
@@ -334,7 +331,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -342,7 +339,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -428,13 +425,13 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -520,8 +517,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -547,34 +544,34 @@
         <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,7 +588,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>2</v>
@@ -606,7 +603,7 @@
         <v>7</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,7 +620,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>3</v>
@@ -638,7 +635,7 @@
         <v>7</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,16 +649,16 @@
         <v>13</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4" s="0" t="s">
         <v>7</v>
@@ -678,42 +675,42 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>14</v>
@@ -724,59 +721,59 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="I7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="K7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>14</v>
@@ -790,97 +787,97 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="0" t="s">
+      <c r="I10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="I11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="K11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="M11" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="I12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="M12" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="I13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="K13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>